<commit_message>
no he terminado, estoy en ello
</commit_message>
<xml_diff>
--- a/Calendario junio julio.xlsx
+++ b/Calendario junio julio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Víctor\Documents\Ingienería informatica\tfg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\victor\universidad\tfm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Revisar entrega del word de propuesta tfg</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>En agosto se sucederan las revisiones como me vayas diciendo</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>PROBLEMAS</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +648,9 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3">
         <v>1</v>
@@ -676,7 +684,9 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3">
         <v>3</v>
@@ -693,7 +703,9 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3">
         <v>4</v>
@@ -745,7 +757,9 @@
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3">
         <v>1</v>
@@ -762,7 +776,9 @@
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3">
         <v>2</v>
@@ -779,7 +795,9 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3">
         <v>3</v>

</xml_diff>